<commit_message>
docgen.hangul.auto_postfix -> docgen.hangul.auto_suffix 로 수정
</commit_message>
<xml_diff>
--- a/Common/doc/docgen/media/docgen_variables.xlsx
+++ b/Common/doc/docgen/media/docgen_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\docgen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA4926-0A3C-40CC-81BC-69CA64E0F223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82671B1-E016-4A86-9C37-2406B245EE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -228,10 +228,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>docgen.hangul.auto_postfix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Enable correction of the Korean suffix after bookmark or property
 - Modify "이/가", "을/를", "은/는" and "와/과" to match the pronunciation.
 (default : true)</t>
@@ -241,6 +237,10 @@
     <t>bookmark 나 property 뒤의 한글 접미사를 올바르게 수정을 활성화
 "이/가", "을/를", "은/는", "와/과" 를 알맞게 수정한다.
 (default : true)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docgen.hangul.auto_suffix</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -722,13 +722,13 @@
     </row>
     <row r="13" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27C0F04-F5AF-48B5-963E-51148E9BECA9}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -887,13 +887,13 @@
     </row>
     <row r="13" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docgen 변수 docgen.bookmark.always_bold 추가
</commit_message>
<xml_diff>
--- a/Common/doc/docgen/media/docgen_variables.xlsx
+++ b/Common/doc/docgen/media/docgen_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\docgen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A2AC0E-3F88-4FC4-A2DB-94042922FB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011174B-9B1B-4343-930B-A7A994255066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8910" yWindow="1275" windowWidth="18495" windowHeight="14265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>Variable</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -275,6 +275,20 @@
   <si>
     <t>표 너비 비율 (0 &lt; 너비_비율 &lt;= 1)
 (기본값 : 1.0, 표에 적용 후 다시 1.0로 리셋됨.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docgen.bookmark.always_bold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blookmark 참조를 항상 굵은 글씨로 표현합니다.
+(기본값 : false)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blookmark text always display in bold.
+(default : false)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -609,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -787,6 +801,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="33" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -796,10 +821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27C0F04-F5AF-48B5-963E-51148E9BECA9}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -974,6 +999,17 @@
         <v>49</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="33" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>